<commit_message>
Implement mse loss function and its derivative
</commit_message>
<xml_diff>
--- a/Experiment/simd_vs_std.xlsx
+++ b/Experiment/simd_vs_std.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\ML\Cortex++\Experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF23852-6FFE-4F68-9309-FEE840FA1018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{13443330-E257-4710-87B2-ABE8052613BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{8F4A0F63-3757-4492-90C0-FF20E63FB1CA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8F4A0F63-3757-4492-90C0-FF20E63FB1CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>AVX-2 (Taylor Series) (ms)</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -72,6 +73,18 @@
   </si>
   <si>
     <t>10240 float in memory (uniform distribution)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Term 0 (1 + x)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Term 1 ( + x^2 * 0.5)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Term 2 (+x^3 / 6)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -79,7 +92,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -94,6 +107,12 @@
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="17.3"/>
+      <color rgb="FF79B8FF"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -118,7 +137,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -127,6 +146,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -442,27 +464,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36308616-6262-4499-907E-534E3D9D008C}">
-  <dimension ref="D8:F18"/>
+  <dimension ref="D8:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="2" max="2" width="11.875" customWidth="1"/>
     <col min="5" max="5" width="13.125" customWidth="1"/>
     <col min="6" max="6" width="17.75" customWidth="1"/>
+    <col min="10" max="10" width="17.75" customWidth="1"/>
+    <col min="11" max="11" width="22.25" customWidth="1"/>
+    <col min="12" max="12" width="25.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="4:6">
       <c r="D8" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="4:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="4:6" ht="36" customHeight="1">
       <c r="E9" s="1" t="s">
         <v>1</v>
       </c>
@@ -470,7 +495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="4:6">
       <c r="D10" t="s">
         <v>2</v>
       </c>
@@ -481,7 +506,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="11" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="4:6">
       <c r="D11" t="s">
         <v>3</v>
       </c>
@@ -492,7 +517,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="12" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="4:6">
       <c r="D12" t="s">
         <v>4</v>
       </c>
@@ -503,7 +528,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="13" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="4:6">
       <c r="D13" t="s">
         <v>5</v>
       </c>
@@ -514,7 +539,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="14" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="4:6">
       <c r="D14" t="s">
         <v>6</v>
       </c>
@@ -525,7 +550,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="15" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="4:6">
       <c r="D15" t="s">
         <v>7</v>
       </c>
@@ -536,7 +561,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="16" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="4:6">
       <c r="D16" t="s">
         <v>8</v>
       </c>
@@ -547,7 +572,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="17" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="4:13">
       <c r="D17" t="s">
         <v>9</v>
       </c>
@@ -558,7 +583,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="18" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="4:13">
       <c r="D18" t="s">
         <v>10</v>
       </c>
@@ -569,6 +594,189 @@
       <c r="F18">
         <f>AVERAGE(F10:F17)</f>
         <v>151.375</v>
+      </c>
+      <c r="G18">
+        <v>4.0016499999999997</v>
+      </c>
+    </row>
+    <row r="22" spans="4:13">
+      <c r="J22" t="s">
+        <v>12</v>
+      </c>
+      <c r="K22" t="s">
+        <v>13</v>
+      </c>
+      <c r="L22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="4:13" ht="22.5">
+      <c r="D23" s="3"/>
+      <c r="I23">
+        <v>0.46529999999999999</v>
+      </c>
+      <c r="J23">
+        <f>1+I23</f>
+        <v>1.4653</v>
+      </c>
+      <c r="K23">
+        <f>J23  + I23 * I23 * 0.5</f>
+        <v>1.573552045</v>
+      </c>
+      <c r="L23">
+        <f>K23 +POWER(I23, 3)</f>
+        <v>1.674291398077</v>
+      </c>
+      <c r="M23">
+        <f>POWER(I23, 3)</f>
+        <v>0.10073935307699999</v>
+      </c>
+    </row>
+    <row r="24" spans="4:13">
+      <c r="I24">
+        <v>0.77610000000000001</v>
+      </c>
+      <c r="J24">
+        <f t="shared" ref="J24:J30" si="0">1+I24</f>
+        <v>1.7761</v>
+      </c>
+      <c r="K24">
+        <f t="shared" ref="K24:K30" si="1">J24  + I24 * I24 * 0.5</f>
+        <v>2.077265605</v>
+      </c>
+      <c r="L24">
+        <f t="shared" ref="L24:L30" si="2">K24 +POWER(I24, 3) / 6</f>
+        <v>2.1551771470135002</v>
+      </c>
+      <c r="M24">
+        <f t="shared" ref="M24:M30" si="3">POWER(I24, 3)</f>
+        <v>0.46746925208099999</v>
+      </c>
+    </row>
+    <row r="25" spans="4:13">
+      <c r="I25">
+        <v>0.70940000000000003</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="0"/>
+        <v>1.7094</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="1"/>
+        <v>1.9610241800000001</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="2"/>
+        <v>2.0205249110973336</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="3"/>
+        <v>0.35700438658400008</v>
+      </c>
+    </row>
+    <row r="26" spans="4:13">
+      <c r="I26">
+        <v>0.57589999999999997</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="0"/>
+        <v>1.5758999999999999</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="1"/>
+        <v>1.7417304049999998</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="2"/>
+        <v>1.773564315079833</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="3"/>
+        <v>0.19100346047899996</v>
+      </c>
+    </row>
+    <row r="27" spans="4:13">
+      <c r="I27">
+        <v>0.19919999999999999</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="0"/>
+        <v>1.1992</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="1"/>
+        <v>1.21904032</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="2"/>
+        <v>1.220357717248</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="3"/>
+        <v>7.904383487999999E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="4:13">
+      <c r="I28">
+        <v>0.78800000000000003</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="0"/>
+        <v>1.788</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="1"/>
+        <v>2.0984720000000001</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="2"/>
+        <v>2.1800226453333336</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="3"/>
+        <v>0.48930387200000008</v>
+      </c>
+    </row>
+    <row r="29" spans="4:13">
+      <c r="I29">
+        <v>0.43159999999999998</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="0"/>
+        <v>1.4316</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="1"/>
+        <v>1.5247392799999999</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="2"/>
+        <v>1.5381389177493332</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="3"/>
+        <v>8.0397826495999983E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="4:13">
+      <c r="I30">
+        <v>0.64910000000000001</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="0"/>
+        <v>1.6491</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="1"/>
+        <v>1.8597654050000001</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="2"/>
+        <v>1.9053463764618335</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="3"/>
+        <v>0.27348582877100003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>